<commit_message>
Update front end visuals. Add rho to Portfolio get greeks method
</commit_message>
<xml_diff>
--- a/ReportSkellie.xlsx
+++ b/ReportSkellie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Razi\Desktop\Projects\RoboAdvisor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E310953-F711-4A80-B693-7DB09C628D93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FD1181-09FD-49A4-A18F-4AA7366427A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12936" windowHeight="7320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,6 +346,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5E99-4DD0-8B72-7FD9D1247056}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -361,6 +366,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5E99-4DD0-8B72-7FD9D1247056}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -376,6 +386,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5E99-4DD0-8B72-7FD9D1247056}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -391,6 +406,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-5E99-4DD0-8B72-7FD9D1247056}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -610,6 +630,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -625,6 +650,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -640,6 +670,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -655,6 +690,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -670,6 +710,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -685,6 +730,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -702,6 +752,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -719,6 +774,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -736,6 +796,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -753,6 +818,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -770,6 +840,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -787,6 +862,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -805,6 +885,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -823,6 +908,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -841,6 +931,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -859,6 +954,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -877,6 +977,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -895,6 +1000,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -912,6 +1022,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -929,6 +1044,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
@@ -946,6 +1066,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="21"/>
@@ -963,6 +1088,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="22"/>
@@ -980,6 +1110,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="23"/>
@@ -997,6 +1132,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="24"/>
@@ -1015,6 +1155,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="25"/>
@@ -1033,6 +1178,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="26"/>
@@ -1051,6 +1201,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-AB48-4D43-923C-468C9EF7BFD6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2817,7 +2972,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2847,7 +3002,7 @@
         <v>6</v>
       </c>
       <c r="J2" s="2">
-        <f>1/27</f>
+        <f t="shared" ref="J2:J28" si="0">1/27</f>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2862,7 +3017,7 @@
         <v>7</v>
       </c>
       <c r="J3" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2877,7 +3032,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2892,7 +3047,7 @@
         <v>9</v>
       </c>
       <c r="J5" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2901,7 +3056,7 @@
         <v>10</v>
       </c>
       <c r="J6" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2910,7 +3065,7 @@
         <v>11</v>
       </c>
       <c r="J7" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2919,7 +3074,7 @@
         <v>12</v>
       </c>
       <c r="J8" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2928,7 +3083,7 @@
         <v>13</v>
       </c>
       <c r="J9" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2937,7 +3092,7 @@
         <v>14</v>
       </c>
       <c r="J10" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2946,7 +3101,7 @@
         <v>15</v>
       </c>
       <c r="J11" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2955,7 +3110,7 @@
         <v>16</v>
       </c>
       <c r="J12" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2964,7 +3119,7 @@
         <v>17</v>
       </c>
       <c r="J13" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2973,7 +3128,7 @@
         <v>18</v>
       </c>
       <c r="J14" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2982,7 +3137,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -2991,7 +3146,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3000,7 +3155,7 @@
         <v>21</v>
       </c>
       <c r="J17" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3009,7 +3164,7 @@
         <v>22</v>
       </c>
       <c r="J18" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3018,7 +3173,7 @@
         <v>23</v>
       </c>
       <c r="J19" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3027,7 +3182,7 @@
         <v>24</v>
       </c>
       <c r="J20" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3036,7 +3191,7 @@
         <v>25</v>
       </c>
       <c r="J21" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3045,7 +3200,7 @@
         <v>26</v>
       </c>
       <c r="J22" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3054,7 +3209,7 @@
         <v>27</v>
       </c>
       <c r="J23" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3063,7 +3218,7 @@
         <v>28</v>
       </c>
       <c r="J24" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3072,7 +3227,7 @@
         <v>29</v>
       </c>
       <c r="J25" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3081,7 +3236,7 @@
         <v>30</v>
       </c>
       <c r="J26" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3090,7 +3245,7 @@
         <v>31</v>
       </c>
       <c r="J27" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -3099,13 +3254,14 @@
         <v>32</v>
       </c>
       <c r="J28" s="2">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3117,7 +3273,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3223,11 +3379,11 @@
         <v>6</v>
       </c>
       <c r="L2" s="5">
-        <f>1/27</f>
+        <f t="shared" ref="L2:M28" si="0">1/27</f>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M2" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N2" s="5">
@@ -3237,11 +3393,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P2" s="5">
-        <f>1/27</f>
+        <f t="shared" ref="P2:Q28" si="1">1/27</f>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q2" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R2" s="8">
@@ -3283,11 +3439,11 @@
         <v>7</v>
       </c>
       <c r="L3" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M3" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N3" s="5">
@@ -3297,11 +3453,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P3" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q3" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R3" s="8">
@@ -3343,11 +3499,11 @@
         <v>8</v>
       </c>
       <c r="L4" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M4" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N4" s="5">
@@ -3357,11 +3513,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P4" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q4" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R4" s="8">
@@ -3403,11 +3559,11 @@
         <v>9</v>
       </c>
       <c r="L5" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M5" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N5" s="5">
@@ -3417,11 +3573,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P5" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q5" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R5" s="8">
@@ -3436,11 +3592,11 @@
         <v>10</v>
       </c>
       <c r="L6" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M6" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N6" s="5">
@@ -3450,11 +3606,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P6" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q6" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R6" s="8">
@@ -3469,11 +3625,11 @@
         <v>11</v>
       </c>
       <c r="L7" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M7" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N7" s="5">
@@ -3483,11 +3639,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P7" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q7" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R7" s="8">
@@ -3502,11 +3658,11 @@
         <v>12</v>
       </c>
       <c r="L8" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M8" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N8" s="5">
@@ -3516,11 +3672,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P8" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q8" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R8" s="8">
@@ -3535,11 +3691,11 @@
         <v>13</v>
       </c>
       <c r="L9" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M9" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N9" s="5">
@@ -3549,11 +3705,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P9" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q9" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R9" s="8">
@@ -3568,11 +3724,11 @@
         <v>14</v>
       </c>
       <c r="L10" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M10" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N10" s="5">
@@ -3582,11 +3738,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P10" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q10" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R10" s="8">
@@ -3601,11 +3757,11 @@
         <v>15</v>
       </c>
       <c r="L11" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M11" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N11" s="5">
@@ -3615,11 +3771,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P11" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q11" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R11" s="8">
@@ -3634,11 +3790,11 @@
         <v>16</v>
       </c>
       <c r="L12" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M12" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N12" s="5">
@@ -3648,11 +3804,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P12" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q12" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R12" s="8">
@@ -3667,11 +3823,11 @@
         <v>17</v>
       </c>
       <c r="L13" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M13" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N13" s="5">
@@ -3681,11 +3837,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P13" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q13" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R13" s="8">
@@ -3700,11 +3856,11 @@
         <v>18</v>
       </c>
       <c r="L14" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M14" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N14" s="5">
@@ -3714,11 +3870,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P14" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q14" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R14" s="8">
@@ -3733,11 +3889,11 @@
         <v>19</v>
       </c>
       <c r="L15" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M15" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N15" s="5">
@@ -3747,11 +3903,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P15" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q15" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R15" s="8">
@@ -3766,11 +3922,11 @@
         <v>20</v>
       </c>
       <c r="L16" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M16" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N16" s="5">
@@ -3780,11 +3936,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P16" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q16" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R16" s="8">
@@ -3799,11 +3955,11 @@
         <v>21</v>
       </c>
       <c r="L17" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M17" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N17" s="5">
@@ -3813,11 +3969,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P17" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q17" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R17" s="8">
@@ -3832,11 +3988,11 @@
         <v>22</v>
       </c>
       <c r="L18" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M18" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N18" s="5">
@@ -3846,11 +4002,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P18" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q18" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R18" s="8">
@@ -3865,11 +4021,11 @@
         <v>23</v>
       </c>
       <c r="L19" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M19" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N19" s="5">
@@ -3879,11 +4035,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P19" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q19" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R19" s="8">
@@ -3898,11 +4054,11 @@
         <v>24</v>
       </c>
       <c r="L20" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M20" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N20" s="5">
@@ -3912,11 +4068,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P20" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q20" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R20" s="8">
@@ -3931,11 +4087,11 @@
         <v>25</v>
       </c>
       <c r="L21" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M21" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N21" s="5">
@@ -3945,11 +4101,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P21" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q21" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R21" s="8">
@@ -3964,11 +4120,11 @@
         <v>26</v>
       </c>
       <c r="L22" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M22" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N22" s="5">
@@ -3978,11 +4134,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P22" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q22" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R22" s="8">
@@ -3997,11 +4153,11 @@
         <v>27</v>
       </c>
       <c r="L23" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M23" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N23" s="5">
@@ -4011,11 +4167,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P23" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q23" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R23" s="8">
@@ -4030,11 +4186,11 @@
         <v>28</v>
       </c>
       <c r="L24" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M24" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N24" s="5">
@@ -4044,11 +4200,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P24" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q24" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R24" s="8">
@@ -4063,11 +4219,11 @@
         <v>29</v>
       </c>
       <c r="L25" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M25" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N25" s="5">
@@ -4077,11 +4233,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P25" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q25" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R25" s="8">
@@ -4096,11 +4252,11 @@
         <v>30</v>
       </c>
       <c r="L26" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M26" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N26" s="5">
@@ -4110,11 +4266,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P26" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q26" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R26" s="8">
@@ -4129,11 +4285,11 @@
         <v>31</v>
       </c>
       <c r="L27" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M27" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N27" s="5">
@@ -4143,11 +4299,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P27" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q27" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R27" s="8">
@@ -4162,11 +4318,11 @@
         <v>32</v>
       </c>
       <c r="L28" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="M28" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="N28" s="5">
@@ -4176,11 +4332,11 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="P28" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="Q28" s="5">
-        <f>1/27</f>
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="R28" s="8">
@@ -4203,7 +4359,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4256,15 +4412,15 @@
         <v>6</v>
       </c>
       <c r="H2" s="5">
-        <f>1/27</f>
+        <f t="shared" ref="H2:J28" si="0">1/27</f>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I2" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J2" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4285,15 +4441,15 @@
         <v>7</v>
       </c>
       <c r="H3" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I3" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J3" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4314,15 +4470,15 @@
         <v>8</v>
       </c>
       <c r="H4" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I4" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J4" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4343,15 +4499,15 @@
         <v>9</v>
       </c>
       <c r="H5" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I5" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J5" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4360,15 +4516,15 @@
         <v>10</v>
       </c>
       <c r="H6" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I6" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J6" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4377,15 +4533,15 @@
         <v>11</v>
       </c>
       <c r="H7" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I7" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J7" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4394,15 +4550,15 @@
         <v>12</v>
       </c>
       <c r="H8" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I8" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J8" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4411,15 +4567,15 @@
         <v>13</v>
       </c>
       <c r="H9" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I9" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J9" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4428,15 +4584,15 @@
         <v>14</v>
       </c>
       <c r="H10" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I10" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J10" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4445,15 +4601,15 @@
         <v>15</v>
       </c>
       <c r="H11" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I11" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J11" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4462,15 +4618,15 @@
         <v>16</v>
       </c>
       <c r="H12" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I12" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J12" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4479,15 +4635,15 @@
         <v>17</v>
       </c>
       <c r="H13" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I13" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J13" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4496,15 +4652,15 @@
         <v>18</v>
       </c>
       <c r="H14" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I14" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J14" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4513,15 +4669,15 @@
         <v>19</v>
       </c>
       <c r="H15" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I15" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J15" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4530,15 +4686,15 @@
         <v>20</v>
       </c>
       <c r="H16" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I16" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J16" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4547,15 +4703,15 @@
         <v>21</v>
       </c>
       <c r="H17" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I17" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J17" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4564,15 +4720,15 @@
         <v>22</v>
       </c>
       <c r="H18" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I18" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J18" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4581,15 +4737,15 @@
         <v>23</v>
       </c>
       <c r="H19" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I19" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J19" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4598,15 +4754,15 @@
         <v>24</v>
       </c>
       <c r="H20" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I20" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J20" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4615,15 +4771,15 @@
         <v>25</v>
       </c>
       <c r="H21" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I21" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J21" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4632,15 +4788,15 @@
         <v>26</v>
       </c>
       <c r="H22" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I22" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J22" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4649,15 +4805,15 @@
         <v>27</v>
       </c>
       <c r="H23" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I23" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J23" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4666,15 +4822,15 @@
         <v>28</v>
       </c>
       <c r="H24" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I24" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J24" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4683,15 +4839,15 @@
         <v>29</v>
       </c>
       <c r="H25" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I25" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J25" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4700,15 +4856,15 @@
         <v>30</v>
       </c>
       <c r="H26" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I26" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J26" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4717,15 +4873,15 @@
         <v>31</v>
       </c>
       <c r="H27" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I27" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J27" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -4734,15 +4890,15 @@
         <v>32</v>
       </c>
       <c r="H28" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="I28" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="J28" s="5">
-        <f>1/27</f>
+        <f t="shared" si="0"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>

</xml_diff>